<commit_message>
Validate and fix Ao5 / Mo3
</commit_message>
<xml_diff>
--- a/data/2020-01-28/Senior Cubers Worldwide - Weekly Competition - 2020-01-28.xlsx
+++ b/data/2020-01-28/Senior Cubers Worldwide - Weekly Competition - 2020-01-28.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\scw-weekly-comp\data\2020-02-03\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\scw-comp\data\2020-01-28\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF41BE8-1C58-48EC-A21B-D1DF844ECCF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8896EBAA-95C1-41F4-8A72-C1920F16D841}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -201,9 +201,6 @@
     <t>Jo Cocco</t>
   </si>
   <si>
-    <t>1:19.00</t>
-  </si>
-  <si>
     <t>1:01.04</t>
   </si>
   <si>
@@ -220,6 +217,9 @@
   </si>
   <si>
     <t>Grzegorz Pacewicz</t>
+  </si>
+  <si>
+    <t>1:19.47</t>
   </si>
 </sst>
 </file>
@@ -288,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -327,6 +327,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -548,7 +551,7 @@
   <dimension ref="A1:I1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F25" sqref="F25:H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -733,7 +736,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>21</v>
@@ -980,7 +983,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>21</v>
@@ -1116,7 +1119,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>21</v>
@@ -1148,21 +1151,21 @@
       <c r="C23" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="12" t="s">
-        <v>57</v>
+      <c r="D23" s="18" t="s">
+        <v>63</v>
       </c>
       <c r="E23" s="10"/>
       <c r="F23" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G23" s="15">
         <v>56.27</v>
       </c>
       <c r="H23" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="I23" s="13" t="s">
         <v>59</v>
-      </c>
-      <c r="I23" s="13" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Rename Deansie to Jamie Brady (Deansie)
</commit_message>
<xml_diff>
--- a/data/2020-01-28/Senior Cubers Worldwide - Weekly Competition - 2020-01-28.xlsx
+++ b/data/2020-01-28/Senior Cubers Worldwide - Weekly Competition - 2020-01-28.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\scw-comp\data\2020-01-28\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8896EBAA-95C1-41F4-8A72-C1920F16D841}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420D3594-BBD0-4C0D-A3AF-D7132939F216}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -156,9 +156,6 @@
     <t>https://www.facebook.com/100017395687396/videos/558635781392940/</t>
   </si>
   <si>
-    <t>Deansie Brady</t>
-  </si>
-  <si>
     <t>https://www.facebook.com/Magnacube.askme/videos/1047021635647834/</t>
   </si>
   <si>
@@ -220,6 +217,9 @@
   </si>
   <si>
     <t>1:19.47</t>
+  </si>
+  <si>
+    <t>Jamie Brady (Deansie)</t>
   </si>
 </sst>
 </file>
@@ -237,29 +237,34 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -551,7 +556,7 @@
   <dimension ref="A1:I1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25:H25"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -736,7 +741,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>21</v>
@@ -955,8 +960,8 @@
       <c r="A16" s="10">
         <v>13</v>
       </c>
-      <c r="B16" s="11" t="s">
-        <v>42</v>
+      <c r="B16" s="17" t="s">
+        <v>63</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>32</v>
@@ -975,7 +980,7 @@
         <v>21.11</v>
       </c>
       <c r="I16" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
@@ -983,7 +988,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>21</v>
@@ -1002,7 +1007,7 @@
         <v>27.77</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
@@ -1010,7 +1015,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>32</v>
@@ -1029,7 +1034,7 @@
         <v>31.06</v>
       </c>
       <c r="I18" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
@@ -1037,7 +1042,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>18</v>
@@ -1056,7 +1061,7 @@
         <v>28.16</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
@@ -1064,7 +1069,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>21</v>
@@ -1083,7 +1088,7 @@
         <v>34.15</v>
       </c>
       <c r="I20" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
@@ -1091,7 +1096,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>21</v>
@@ -1111,7 +1116,7 @@
         <v>41.19</v>
       </c>
       <c r="I21" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
@@ -1119,7 +1124,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>21</v>
@@ -1132,13 +1137,13 @@
         <v>43.32</v>
       </c>
       <c r="G22" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="H22" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="H22" s="12" t="s">
+      <c r="I22" s="13" t="s">
         <v>54</v>
-      </c>
-      <c r="I22" s="13" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
@@ -1146,26 +1151,26 @@
         <v>20</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>21</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E23" s="10"/>
       <c r="F23" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G23" s="15">
         <v>56.27</v>
       </c>
       <c r="H23" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="I23" s="13" t="s">
         <v>58</v>
-      </c>
-      <c r="I23" s="13" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">

</xml_diff>